<commit_message>
Complete impact from maintenance¨
</commit_message>
<xml_diff>
--- a/data/Bostadsarea per län.xlsx
+++ b/data/Bostadsarea per län.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasGustafsson\Jupyter Notebooks\climate-impact-re-se\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D180312C-19CF-408A-BB65-38F824C47B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0082393C-4891-49C8-B8A2-C5A1CC5C0048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,16 +769,6 @@
         <v>9957</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="2">
-        <f>SUM(B2:B22)</f>
-        <v>208969</v>
-      </c>
-      <c r="C23" s="2">
-        <f>SUM(C2:C22)</f>
-        <v>184837</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>

</xml_diff>